<commit_message>
adding last workbook version
</commit_message>
<xml_diff>
--- a/project_management/project_tracking_gnlg2.xlsx
+++ b/project_management/project_tracking_gnlg2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivo/repositories/GNLG2/project_management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{00F355F3-2347-3E46-A28C-C8883C65C78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5756B8B9-8C8A-8C47-B121-1BAB590B5C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tab" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="23" r:id="rId3"/>
+    <pivotCache cacheId="70" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="405" uniqueCount="72">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="469" uniqueCount="77">
   <si>
     <t>CM</t>
   </si>
@@ -245,6 +245,21 @@
   </si>
   <si>
     <t>Workbook v4 corrections</t>
+  </si>
+  <si>
+    <t>Update the team on laravel project + development</t>
+  </si>
+  <si>
+    <t>Description on how to do project tracking by ICC</t>
+  </si>
+  <si>
+    <t>Workbook redaction</t>
+  </si>
+  <si>
+    <t>Workbook redaction finalisation</t>
+  </si>
+  <si>
+    <t>Laravel development</t>
   </si>
 </sst>
 </file>
@@ -386,7 +401,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -439,6 +454,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC0C0C0"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -652,7 +673,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -683,14 +704,8 @@
     <xf numFmtId="0" fontId="14" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" pivotButton="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -724,16 +739,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="17" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -753,7 +759,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -798,13 +823,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDateIso="2021-11-19T16:09:24.87000030465423825" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="188" xr:uid="{33C243A7-C20F-9A41-84D4-AFCEDFA037F4}">
+<pivotCacheDefinition xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDateIso="2021-11-26T16:52:48.529999698512255850" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="188" xr:uid="{33C243A7-C20F-9A41-84D4-AFCEDFA037F4}">
   <cacheSource type="worksheet">
     <worksheetSource ref="C34:G222" sheet="Tab"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2021-10-22T00:00:00" maxDate="2021-11-20T00:00:00" count="16">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2021-10-22T00:00:00" maxDate="2021-11-27T00:00:00" count="19">
         <d v="2021-10-22T00:00:00"/>
         <d v="2021-10-27T00:00:00"/>
         <d v="2021-10-28T00:00:00"/>
@@ -820,6 +845,9 @@
         <d v="2021-11-17T00:00:00"/>
         <d v="2021-11-18T00:00:00"/>
         <d v="2021-11-19T00:00:00"/>
+        <d v="2021-11-24T00:00:00"/>
+        <d v="2021-11-25T00:00:00"/>
+        <d v="2021-11-26T00:00:00"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -1672,510 +1700,510 @@
   </r>
   <r>
     <x v="15"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="0.3"/>
+    <s v="Metting with M. Oudot"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="0.3"/>
+    <s v="Metting with M. Oudot"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.3"/>
+    <s v="Metting with M. Oudot"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="0.3"/>
+    <s v="Metting with M. Oudot"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="0.3"/>
+    <s v="Metting with M. Oudot"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="0.7"/>
+    <s v="Update the team on laravel project + development"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="0.7"/>
+    <s v="Update the team on laravel project + development"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="0.7"/>
+    <s v="Update the team on laravel project + development"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.7"/>
+    <s v="Update the team on laravel project + development"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="0.7"/>
+    <s v="Update the team on laravel project + development"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1"/>
+    <s v="Workbook redaction"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1"/>
+    <s v="Workbook redaction"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1"/>
+    <s v="Workbook redaction"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1"/>
+    <s v="Workbook redaction"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="0.5"/>
+    <s v="Laravel development"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="0.5"/>
+    <s v="Laravel development"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.5"/>
+    <s v="Laravel development"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="0.5"/>
+    <s v="Laravel development"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="0.3"/>
+    <s v="Laravel development"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="0.8"/>
+    <s v="Workbook redaction finalisation"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.2"/>
+    <s v="Project tracking reporting"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="0.2"/>
+    <s v="Description on how to do project tracking by ICC"/>
+  </r>
+  <r>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="15"/>
+    <x v="18"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
@@ -2185,11 +2213,11 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{56ABA1B9-0D18-E44D-8AA9-6D65D511342F}" name="DataPilot1" cacheId="23" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" enableDrill="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" compact="0" compactData="0">
-  <location ref="A3:G11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{56ABA1B9-0D18-E44D-8AA9-6D65D511342F}" name="DataPilot1" cacheId="70" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" enableDrill="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" compact="0" compactData="0">
+  <location ref="A3:G9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="5">
     <pivotField axis="axisPage" compact="0" outline="0" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="17">
+      <items count="20">
         <item h="1" x="0"/>
         <item h="1" x="1"/>
         <item h="1" x="2"/>
@@ -2198,14 +2226,17 @@
         <item h="1" x="6"/>
         <item h="1" x="7"/>
         <item h="1" x="8"/>
-        <item h="1" x="15"/>
+        <item h="1" x="18"/>
         <item h="1" x="5"/>
         <item h="1" x="10"/>
         <item h="1" x="11"/>
         <item h="1" x="9"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
+        <item h="1" x="12"/>
+        <item h="1" x="13"/>
+        <item h="1" x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2240,7 +2271,7 @@
   <rowFields count="1">
     <field x="2"/>
   </rowFields>
-  <rowItems count="7">
+  <rowItems count="5">
     <i>
       <x/>
     </i>
@@ -2252,12 +2283,6 @@
     </i>
     <i>
       <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="9"/>
     </i>
     <i t="grand">
       <x/>
@@ -2600,8 +2625,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="D150" sqref="D150"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="E166" sqref="E166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2727,42 +2752,42 @@
       </c>
     </row>
     <row r="17" spans="3:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="43" t="s">
+      <c r="D17" s="38" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="18" spans="3:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="43" t="s">
+      <c r="D18" s="38" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C19" s="43" t="s">
+      <c r="C19" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="D19" s="43" t="s">
+      <c r="D19" s="38" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C20" s="43" t="s">
+      <c r="C20" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="43" t="s">
+      <c r="D20" s="38" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C21" s="43" t="s">
+      <c r="C21" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="D21" s="43" t="s">
+      <c r="D21" s="38" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2789,1853 +2814,1853 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C35" s="28" t="d">
+      <c r="C35" s="26" t="d">
         <v>2021-10-22</v>
       </c>
-      <c r="D35" s="29" t="s">
+      <c r="D35" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="E35" s="29" t="s">
+      <c r="E35" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F35" s="29">
+      <c r="F35" s="27">
         <v>0.1</v>
       </c>
-      <c r="G35" s="29" t="s">
+      <c r="G35" s="27" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C36" s="28" t="d">
+      <c r="C36" s="26" t="d">
         <v>2021-10-22</v>
       </c>
-      <c r="D36" s="29" t="s">
+      <c r="D36" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E36" s="29" t="s">
+      <c r="E36" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F36" s="29">
+      <c r="F36" s="27">
         <v>0.1</v>
       </c>
-      <c r="G36" s="29" t="s">
+      <c r="G36" s="27" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C37" s="28" t="d">
+      <c r="C37" s="26" t="d">
         <v>2021-10-22</v>
       </c>
-      <c r="D37" s="29" t="s">
+      <c r="D37" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="29" t="s">
+      <c r="E37" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F37" s="29">
+      <c r="F37" s="27">
         <v>0.1</v>
       </c>
-      <c r="G37" s="29" t="s">
+      <c r="G37" s="27" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C38" s="28" t="d">
+      <c r="C38" s="26" t="d">
         <v>2021-10-22</v>
       </c>
-      <c r="D38" s="29" t="s">
+      <c r="D38" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E38" s="29" t="s">
+      <c r="E38" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F38" s="29">
+      <c r="F38" s="27">
         <v>0.1</v>
       </c>
-      <c r="G38" s="29" t="s">
+      <c r="G38" s="27" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C39" s="28" t="d">
+      <c r="C39" s="26" t="d">
         <v>2021-10-22</v>
       </c>
-      <c r="D39" s="29" t="s">
+      <c r="D39" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E39" s="29" t="s">
+      <c r="E39" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F39" s="29">
+      <c r="F39" s="27">
         <v>0.1</v>
       </c>
-      <c r="G39" s="29" t="s">
+      <c r="G39" s="27" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C40" s="28" t="d">
+      <c r="C40" s="26" t="d">
         <v>2021-10-22</v>
       </c>
-      <c r="D40" s="29" t="s">
+      <c r="D40" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="E40" s="29" t="s">
+      <c r="E40" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F40" s="29">
+      <c r="F40" s="27">
         <v>0.3</v>
       </c>
-      <c r="G40" s="30" t="s">
+      <c r="G40" s="28" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C41" s="28" t="d">
+      <c r="C41" s="26" t="d">
         <v>2021-10-22</v>
       </c>
-      <c r="D41" s="29" t="s">
+      <c r="D41" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E41" s="29" t="s">
+      <c r="E41" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F41" s="29">
+      <c r="F41" s="27">
         <v>0.3</v>
       </c>
-      <c r="G41" s="30" t="s">
+      <c r="G41" s="28" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C42" s="28" t="d">
+      <c r="C42" s="26" t="d">
         <v>2021-10-22</v>
       </c>
-      <c r="D42" s="29" t="s">
+      <c r="D42" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="29" t="s">
+      <c r="E42" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F42" s="29">
+      <c r="F42" s="27">
         <v>0.3</v>
       </c>
-      <c r="G42" s="30" t="s">
+      <c r="G42" s="28" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C43" s="28" t="d">
+      <c r="C43" s="26" t="d">
         <v>2021-10-22</v>
       </c>
-      <c r="D43" s="29" t="s">
+      <c r="D43" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E43" s="29" t="s">
+      <c r="E43" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F43" s="29">
+      <c r="F43" s="27">
         <v>0.3</v>
       </c>
-      <c r="G43" s="30" t="s">
+      <c r="G43" s="28" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C44" s="28" t="d">
+      <c r="C44" s="26" t="d">
         <v>2021-10-22</v>
       </c>
-      <c r="D44" s="29" t="s">
+      <c r="D44" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E44" s="29" t="s">
+      <c r="E44" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F44" s="29">
+      <c r="F44" s="27">
         <v>0.3</v>
       </c>
-      <c r="G44" s="30" t="s">
+      <c r="G44" s="28" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C45" s="28" t="d">
+      <c r="C45" s="26" t="d">
         <v>2021-10-22</v>
       </c>
-      <c r="D45" s="29" t="s">
+      <c r="D45" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="E45" s="29" t="s">
+      <c r="E45" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F45" s="29">
+      <c r="F45" s="27">
         <v>0.4</v>
       </c>
-      <c r="G45" s="29" t="s">
+      <c r="G45" s="27" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C46" s="28" t="d">
+      <c r="C46" s="26" t="d">
         <v>2021-10-22</v>
       </c>
-      <c r="D46" s="29" t="s">
+      <c r="D46" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E46" s="29" t="s">
+      <c r="E46" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F46" s="29">
+      <c r="F46" s="27">
         <v>0.4</v>
       </c>
-      <c r="G46" s="29" t="s">
+      <c r="G46" s="27" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C47" s="28" t="d">
+      <c r="C47" s="26" t="d">
         <v>2021-10-22</v>
       </c>
-      <c r="D47" s="29" t="s">
+      <c r="D47" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E47" s="29" t="s">
+      <c r="E47" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F47" s="29">
+      <c r="F47" s="27">
         <v>0.4</v>
       </c>
-      <c r="G47" s="29" t="s">
+      <c r="G47" s="27" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C48" s="28" t="d">
+      <c r="C48" s="26" t="d">
         <v>2021-10-22</v>
       </c>
-      <c r="D48" s="29" t="s">
+      <c r="D48" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E48" s="29" t="s">
+      <c r="E48" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F48" s="29">
+      <c r="F48" s="27">
         <v>0.4</v>
       </c>
-      <c r="G48" s="29" t="s">
+      <c r="G48" s="27" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C49" s="28" t="d">
+      <c r="C49" s="26" t="d">
         <v>2021-10-22</v>
       </c>
-      <c r="D49" s="29" t="s">
+      <c r="D49" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E49" s="29" t="s">
+      <c r="E49" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F49" s="29">
+      <c r="F49" s="27">
         <v>0.4</v>
       </c>
-      <c r="G49" s="29" t="s">
+      <c r="G49" s="27" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C50" s="28" t="d">
+      <c r="C50" s="26" t="d">
         <v>2021-10-27</v>
       </c>
-      <c r="D50" s="29" t="s">
+      <c r="D50" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="E50" s="29" t="s">
+      <c r="E50" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F50" s="29">
+      <c r="F50" s="27">
         <v>0.3</v>
       </c>
-      <c r="G50" s="29" t="s">
+      <c r="G50" s="27" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C51" s="28" t="d">
+      <c r="C51" s="26" t="d">
         <v>2021-10-27</v>
       </c>
-      <c r="D51" s="29" t="s">
+      <c r="D51" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E51" s="29" t="s">
+      <c r="E51" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F51" s="29">
+      <c r="F51" s="27">
         <v>0.3</v>
       </c>
-      <c r="G51" s="29" t="s">
+      <c r="G51" s="27" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C52" s="28" t="d">
+      <c r="C52" s="26" t="d">
         <v>2021-10-27</v>
       </c>
-      <c r="D52" s="29" t="s">
+      <c r="D52" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E52" s="29" t="s">
+      <c r="E52" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F52" s="29">
+      <c r="F52" s="27">
         <v>0.3</v>
       </c>
-      <c r="G52" s="29" t="s">
+      <c r="G52" s="27" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C53" s="28" t="d">
+      <c r="C53" s="26" t="d">
         <v>2021-10-27</v>
       </c>
-      <c r="D53" s="29" t="s">
+      <c r="D53" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E53" s="29" t="s">
+      <c r="E53" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F53" s="29">
+      <c r="F53" s="27">
         <v>0.3</v>
       </c>
-      <c r="G53" s="29" t="s">
+      <c r="G53" s="27" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C54" s="28" t="d">
+      <c r="C54" s="26" t="d">
         <v>2021-10-27</v>
       </c>
-      <c r="D54" s="30" t="s">
+      <c r="D54" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E54" s="29" t="s">
+      <c r="E54" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F54" s="29">
+      <c r="F54" s="27">
         <v>0.3</v>
       </c>
-      <c r="G54" s="30" t="s">
+      <c r="G54" s="28" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C55" s="31" t="d">
+      <c r="C55" s="29" t="d">
         <v>2021-10-28</v>
       </c>
-      <c r="D55" s="30" t="s">
+      <c r="D55" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E55" s="30" t="s">
+      <c r="E55" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F55" s="29">
+      <c r="F55" s="27">
         <v>0.45</v>
       </c>
-      <c r="G55" s="30" t="s">
+      <c r="G55" s="28" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C56" s="31" t="d">
+      <c r="C56" s="29" t="d">
         <v>2021-10-28</v>
       </c>
-      <c r="D56" s="30" t="s">
+      <c r="D56" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E56" s="30" t="s">
+      <c r="E56" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F56" s="29">
+      <c r="F56" s="27">
         <v>0.45</v>
       </c>
-      <c r="G56" s="30" t="s">
+      <c r="G56" s="28" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C57" s="31" t="d">
+      <c r="C57" s="29" t="d">
         <v>2021-10-28</v>
       </c>
-      <c r="D57" s="30" t="s">
+      <c r="D57" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E57" s="30" t="s">
+      <c r="E57" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F57" s="29">
+      <c r="F57" s="27">
         <v>0.45</v>
       </c>
-      <c r="G57" s="30" t="s">
+      <c r="G57" s="28" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C58" s="31" t="d">
+      <c r="C58" s="29" t="d">
         <v>2021-10-28</v>
       </c>
-      <c r="D58" s="30" t="s">
+      <c r="D58" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E58" s="30" t="s">
+      <c r="E58" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F58" s="29">
+      <c r="F58" s="27">
         <v>0.45</v>
       </c>
-      <c r="G58" s="30" t="s">
+      <c r="G58" s="28" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C59" s="31" t="d">
+      <c r="C59" s="29" t="d">
         <v>2021-10-28</v>
       </c>
-      <c r="D59" s="30" t="s">
+      <c r="D59" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="E59" s="30" t="s">
+      <c r="E59" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F59" s="29">
+      <c r="F59" s="27">
         <v>0.45</v>
       </c>
-      <c r="G59" s="30" t="s">
+      <c r="G59" s="28" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="60" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C60" s="28" t="d">
+      <c r="C60" s="26" t="d">
         <v>2021-10-29</v>
       </c>
-      <c r="D60" s="29" t="s">
+      <c r="D60" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="E60" s="29" t="s">
+      <c r="E60" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F60" s="29">
+      <c r="F60" s="27">
         <v>0.1</v>
       </c>
-      <c r="G60" s="29" t="s">
+      <c r="G60" s="27" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C61" s="28" t="d">
+      <c r="C61" s="26" t="d">
         <v>2021-10-29</v>
       </c>
-      <c r="D61" s="29" t="s">
+      <c r="D61" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E61" s="29" t="s">
+      <c r="E61" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F61" s="29">
+      <c r="F61" s="27">
         <v>0.1</v>
       </c>
-      <c r="G61" s="29" t="s">
+      <c r="G61" s="27" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C62" s="28" t="d">
+      <c r="C62" s="26" t="d">
         <v>2021-10-29</v>
       </c>
-      <c r="D62" s="29" t="s">
+      <c r="D62" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E62" s="29" t="s">
+      <c r="E62" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F62" s="29">
+      <c r="F62" s="27">
         <v>0.1</v>
       </c>
-      <c r="G62" s="29" t="s">
+      <c r="G62" s="27" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C63" s="28" t="d">
+      <c r="C63" s="26" t="d">
         <v>2021-10-29</v>
       </c>
-      <c r="D63" s="29" t="s">
+      <c r="D63" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E63" s="29" t="s">
+      <c r="E63" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F63" s="29">
+      <c r="F63" s="27">
         <v>0.1</v>
       </c>
-      <c r="G63" s="29" t="s">
+      <c r="G63" s="27" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C64" s="28" t="d">
+      <c r="C64" s="26" t="d">
         <v>2021-10-29</v>
       </c>
-      <c r="D64" s="29" t="s">
+      <c r="D64" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E64" s="29" t="s">
+      <c r="E64" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F64" s="29">
+      <c r="F64" s="27">
         <v>0.1</v>
       </c>
-      <c r="G64" s="29" t="s">
+      <c r="G64" s="27" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="65" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="C65" s="31" t="d">
+      <c r="C65" s="29" t="d">
         <v>2021-10-28</v>
       </c>
-      <c r="D65" s="30" t="s">
+      <c r="D65" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E65" s="30" t="s">
+      <c r="E65" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F65" s="29">
+      <c r="F65" s="27">
         <v>0.5</v>
       </c>
-      <c r="G65" s="30" t="s">
+      <c r="G65" s="28" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="66" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="C66" s="31" t="d">
+      <c r="C66" s="29" t="d">
         <v>2021-10-28</v>
       </c>
-      <c r="D66" s="30" t="s">
+      <c r="D66" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E66" s="30" t="s">
+      <c r="E66" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F66" s="29">
+      <c r="F66" s="27">
         <v>0.5</v>
       </c>
-      <c r="G66" s="30" t="s">
+      <c r="G66" s="28" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="67" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="C67" s="31" t="d">
+      <c r="C67" s="29" t="d">
         <v>2021-10-28</v>
       </c>
-      <c r="D67" s="30" t="s">
+      <c r="D67" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E67" s="30" t="s">
+      <c r="E67" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F67" s="29">
+      <c r="F67" s="27">
         <v>0.5</v>
       </c>
-      <c r="G67" s="30" t="s">
+      <c r="G67" s="28" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="68" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="C68" s="31" t="d">
+      <c r="C68" s="29" t="d">
         <v>2021-10-28</v>
       </c>
-      <c r="D68" s="30" t="s">
+      <c r="D68" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E68" s="30" t="s">
+      <c r="E68" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F68" s="29">
+      <c r="F68" s="27">
         <v>0.5</v>
       </c>
-      <c r="G68" s="30" t="s">
+      <c r="G68" s="28" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="69" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="C69" s="31" t="d">
+      <c r="C69" s="29" t="d">
         <v>2021-10-28</v>
       </c>
-      <c r="D69" s="30" t="s">
+      <c r="D69" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="E69" s="30" t="s">
+      <c r="E69" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F69" s="29">
+      <c r="F69" s="27">
         <v>0.5</v>
       </c>
-      <c r="G69" s="30" t="s">
+      <c r="G69" s="28" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="70" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="C70" s="28" t="d">
+      <c r="C70" s="26" t="d">
         <v>2021-10-29</v>
       </c>
-      <c r="D70" s="29" t="s">
+      <c r="D70" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="E70" s="29" t="s">
+      <c r="E70" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F70" s="29">
+      <c r="F70" s="27">
         <v>0.4</v>
       </c>
-      <c r="G70" s="29" t="s">
+      <c r="G70" s="27" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="71" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="C71" s="28" t="d">
+      <c r="C71" s="26" t="d">
         <v>2021-10-29</v>
       </c>
-      <c r="D71" s="29" t="s">
+      <c r="D71" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E71" s="29" t="s">
+      <c r="E71" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F71" s="29">
+      <c r="F71" s="27">
         <v>0.4</v>
       </c>
-      <c r="G71" s="29" t="s">
+      <c r="G71" s="27" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="72" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="C72" s="28" t="d">
+      <c r="C72" s="26" t="d">
         <v>2021-10-29</v>
       </c>
-      <c r="D72" s="29" t="s">
+      <c r="D72" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E72" s="29" t="s">
+      <c r="E72" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F72" s="29">
+      <c r="F72" s="27">
         <v>0.45</v>
       </c>
-      <c r="G72" s="29" t="s">
+      <c r="G72" s="27" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="73" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="C73" s="28" t="d">
+      <c r="C73" s="26" t="d">
         <v>2021-10-29</v>
       </c>
-      <c r="D73" s="29" t="s">
+      <c r="D73" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E73" s="29" t="s">
+      <c r="E73" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F73" s="29">
+      <c r="F73" s="27">
         <v>0.4</v>
       </c>
-      <c r="G73" s="29" t="s">
+      <c r="G73" s="27" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="74" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="C74" s="31" t="d">
+      <c r="C74" s="29" t="d">
         <v>2021-10-29</v>
       </c>
-      <c r="D74" s="30" t="s">
+      <c r="D74" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="E74" s="29" t="s">
+      <c r="E74" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F74" s="29">
+      <c r="F74" s="27">
         <v>0.4</v>
       </c>
-      <c r="G74" s="29" t="s">
+      <c r="G74" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="I74" s="36"/>
-      <c r="J74" s="37"/>
-      <c r="K74" s="37"/>
-      <c r="L74" s="38"/>
-      <c r="M74" s="37"/>
+      <c r="I74" s="34"/>
+      <c r="J74" s="35"/>
+      <c r="K74" s="35"/>
+      <c r="L74" s="36"/>
+      <c r="M74" s="35"/>
     </row>
     <row r="75" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="C75" s="28" t="d">
+      <c r="C75" s="26" t="d">
         <v>2021-10-29</v>
       </c>
-      <c r="D75" s="29" t="s">
+      <c r="D75" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E75" s="29" t="s">
+      <c r="E75" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F75" s="29">
+      <c r="F75" s="27">
         <v>0.25</v>
       </c>
-      <c r="G75" s="29" t="s">
+      <c r="G75" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="I75" s="36"/>
-      <c r="J75" s="37"/>
-      <c r="K75" s="37"/>
-      <c r="L75" s="38"/>
-      <c r="M75" s="37"/>
+      <c r="I75" s="34"/>
+      <c r="J75" s="35"/>
+      <c r="K75" s="35"/>
+      <c r="L75" s="36"/>
+      <c r="M75" s="35"/>
     </row>
     <row r="76" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="C76" s="28" t="d">
+      <c r="C76" s="26" t="d">
         <v>2021-11-01</v>
       </c>
-      <c r="D76" s="29" t="s">
+      <c r="D76" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E76" s="29" t="s">
+      <c r="E76" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F76" s="29">
+      <c r="F76" s="27">
         <v>0.5</v>
       </c>
-      <c r="G76" s="29" t="s">
+      <c r="G76" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="I76" s="36"/>
-      <c r="J76" s="37"/>
-      <c r="K76" s="37"/>
-      <c r="L76" s="38"/>
-      <c r="M76" s="37"/>
+      <c r="I76" s="34"/>
+      <c r="J76" s="35"/>
+      <c r="K76" s="35"/>
+      <c r="L76" s="36"/>
+      <c r="M76" s="35"/>
     </row>
     <row r="77" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="C77" s="32" t="d">
+      <c r="C77" s="30" t="d">
         <v>2021-11-02</v>
       </c>
-      <c r="D77" s="30" t="s">
+      <c r="D77" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E77" s="30" t="s">
+      <c r="E77" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F77" s="33">
+      <c r="F77" s="31">
         <v>1</v>
       </c>
-      <c r="G77" s="30" t="s">
+      <c r="G77" s="28" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="78" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="C78" s="32" t="d">
+      <c r="C78" s="30" t="d">
         <v>2021-11-02</v>
       </c>
-      <c r="D78" s="30" t="s">
+      <c r="D78" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="E78" s="30" t="s">
+      <c r="E78" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F78" s="33">
+      <c r="F78" s="31">
         <v>0.8</v>
       </c>
-      <c r="G78" s="30" t="s">
+      <c r="G78" s="28" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="79" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="C79" s="32" t="d">
+      <c r="C79" s="30" t="d">
         <v>2021-11-02</v>
       </c>
-      <c r="D79" s="30" t="s">
+      <c r="D79" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E79" s="30" t="s">
+      <c r="E79" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F79" s="33">
+      <c r="F79" s="31">
         <v>1</v>
       </c>
-      <c r="G79" s="30" t="s">
+      <c r="G79" s="28" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="80" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="C80" s="28" t="d">
+      <c r="C80" s="26" t="d">
         <v>2021-11-03</v>
       </c>
-      <c r="D80" s="29" t="s">
+      <c r="D80" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="E80" s="29" t="s">
+      <c r="E80" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F80" s="29">
+      <c r="F80" s="27">
         <v>0.1</v>
       </c>
-      <c r="G80" s="29" t="s">
+      <c r="G80" s="27" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="81" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C81" s="28" t="d">
+      <c r="C81" s="26" t="d">
         <v>2021-11-03</v>
       </c>
-      <c r="D81" s="29" t="s">
+      <c r="D81" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E81" s="29" t="s">
+      <c r="E81" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F81" s="29">
+      <c r="F81" s="27">
         <v>0.1</v>
       </c>
-      <c r="G81" s="29" t="s">
+      <c r="G81" s="27" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="82" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C82" s="28" t="d">
+      <c r="C82" s="26" t="d">
         <v>2021-11-03</v>
       </c>
-      <c r="D82" s="29" t="s">
+      <c r="D82" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E82" s="29" t="s">
+      <c r="E82" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F82" s="29">
+      <c r="F82" s="27">
         <v>0.1</v>
       </c>
-      <c r="G82" s="29" t="s">
+      <c r="G82" s="27" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="83" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C83" s="28" t="d">
+      <c r="C83" s="26" t="d">
         <v>2021-11-03</v>
       </c>
-      <c r="D83" s="29" t="s">
+      <c r="D83" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E83" s="29" t="s">
+      <c r="E83" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F83" s="29">
+      <c r="F83" s="27">
         <v>0.1</v>
       </c>
-      <c r="G83" s="29" t="s">
+      <c r="G83" s="27" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="84" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C84" s="28" t="d">
+      <c r="C84" s="26" t="d">
         <v>2021-11-03</v>
       </c>
-      <c r="D84" s="29" t="s">
+      <c r="D84" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E84" s="29" t="s">
+      <c r="E84" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F84" s="29">
+      <c r="F84" s="27">
         <v>0.1</v>
       </c>
-      <c r="G84" s="29" t="s">
+      <c r="G84" s="27" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="85" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C85" s="32" t="d">
+      <c r="C85" s="30" t="d">
         <v>2021-11-03</v>
       </c>
-      <c r="D85" s="30" t="s">
+      <c r="D85" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="E85" s="30" t="s">
+      <c r="E85" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F85" s="33">
+      <c r="F85" s="31">
         <v>0.3</v>
       </c>
-      <c r="G85" s="30" t="s">
+      <c r="G85" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="86" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C86" s="32" t="d">
+      <c r="C86" s="30" t="d">
         <v>2021-11-03</v>
       </c>
-      <c r="D86" s="30" t="s">
+      <c r="D86" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E86" s="30" t="s">
+      <c r="E86" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F86" s="33">
+      <c r="F86" s="31">
         <v>0.3</v>
       </c>
-      <c r="G86" s="30" t="s">
+      <c r="G86" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="87" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C87" s="32" t="d">
+      <c r="C87" s="30" t="d">
         <v>2021-11-03</v>
       </c>
-      <c r="D87" s="30" t="s">
+      <c r="D87" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E87" s="30" t="s">
+      <c r="E87" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F87" s="33">
+      <c r="F87" s="31">
         <v>0.3</v>
       </c>
-      <c r="G87" s="30" t="s">
+      <c r="G87" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="88" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C88" s="32" t="d">
+      <c r="C88" s="30" t="d">
         <v>2021-11-03</v>
       </c>
-      <c r="D88" s="30" t="s">
+      <c r="D88" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E88" s="30" t="s">
+      <c r="E88" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F88" s="33">
+      <c r="F88" s="31">
         <v>0.3</v>
       </c>
-      <c r="G88" s="30" t="s">
+      <c r="G88" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="89" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C89" s="28" t="d">
+      <c r="C89" s="26" t="d">
         <v>2021-11-03</v>
       </c>
-      <c r="D89" s="29" t="s">
+      <c r="D89" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E89" s="29" t="s">
+      <c r="E89" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F89" s="29">
+      <c r="F89" s="27">
         <v>1</v>
       </c>
-      <c r="G89" s="29" t="s">
+      <c r="G89" s="27" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="90" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C90" s="34" t="d">
+      <c r="C90" s="32" t="d">
         <v>2021-11-04</v>
       </c>
-      <c r="D90" s="35" t="s">
+      <c r="D90" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="E90" s="35" t="s">
+      <c r="E90" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="F90" s="35">
+      <c r="F90" s="33">
         <v>0.4</v>
       </c>
-      <c r="G90" s="35" t="s">
+      <c r="G90" s="33" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="91" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C91" s="32" t="d">
+      <c r="C91" s="30" t="d">
         <v>2021-11-04</v>
       </c>
-      <c r="D91" s="30" t="s">
+      <c r="D91" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E91" s="30" t="s">
+      <c r="E91" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F91" s="33">
+      <c r="F91" s="31">
         <v>0.4</v>
       </c>
-      <c r="G91" s="30" t="s">
+      <c r="G91" s="28" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="92" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C92" s="32" t="d">
+      <c r="C92" s="30" t="d">
         <v>2021-11-04</v>
       </c>
-      <c r="D92" s="30" t="s">
+      <c r="D92" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E92" s="30" t="s">
+      <c r="E92" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F92" s="33">
+      <c r="F92" s="31">
         <v>1</v>
       </c>
-      <c r="G92" s="30" t="s">
+      <c r="G92" s="28" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="93" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C93" s="32" t="d">
+      <c r="C93" s="30" t="d">
         <v>2021-11-04</v>
       </c>
-      <c r="D93" s="30" t="s">
+      <c r="D93" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="E93" s="30" t="s">
+      <c r="E93" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F93" s="33">
+      <c r="F93" s="31">
         <v>1</v>
       </c>
-      <c r="G93" s="30" t="s">
+      <c r="G93" s="28" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="94" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C94" s="32" t="d">
+      <c r="C94" s="30" t="d">
         <v>2021-11-04</v>
       </c>
-      <c r="D94" s="30" t="s">
+      <c r="D94" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E94" s="30" t="s">
+      <c r="E94" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F94" s="33">
+      <c r="F94" s="31">
         <v>1</v>
       </c>
-      <c r="G94" s="30" t="s">
+      <c r="G94" s="28" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="95" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C95" s="32" t="d">
+      <c r="C95" s="30" t="d">
         <v>2021-11-04</v>
       </c>
-      <c r="D95" s="30" t="s">
+      <c r="D95" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E95" s="30" t="s">
+      <c r="E95" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F95" s="33">
+      <c r="F95" s="31">
         <v>1</v>
       </c>
-      <c r="G95" s="30" t="s">
+      <c r="G95" s="28" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="96" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C96" s="32" t="d">
+      <c r="C96" s="30" t="d">
         <v>2021-11-05</v>
       </c>
-      <c r="D96" s="30" t="s">
+      <c r="D96" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E96" s="30" t="s">
+      <c r="E96" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F96" s="33">
+      <c r="F96" s="31">
         <v>1</v>
       </c>
-      <c r="G96" s="30" t="s">
+      <c r="G96" s="28" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="97" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C97" s="32" t="d">
+      <c r="C97" s="30" t="d">
         <v>2021-11-05</v>
       </c>
-      <c r="D97" s="30" t="s">
+      <c r="D97" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="E97" s="30" t="s">
+      <c r="E97" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F97" s="33">
+      <c r="F97" s="31">
         <v>0.3</v>
       </c>
-      <c r="G97" s="30" t="s">
+      <c r="G97" s="28" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C98" s="32" t="d">
+      <c r="C98" s="30" t="d">
         <v>2021-11-05</v>
       </c>
-      <c r="D98" s="30" t="s">
+      <c r="D98" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E98" s="30" t="s">
+      <c r="E98" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F98" s="33">
+      <c r="F98" s="31">
         <v>0.1</v>
       </c>
-      <c r="G98" s="30" t="s">
+      <c r="G98" s="28" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="99" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C99" s="32" t="d">
+      <c r="C99" s="30" t="d">
         <v>2021-11-05</v>
       </c>
-      <c r="D99" s="30" t="s">
+      <c r="D99" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E99" s="30" t="s">
+      <c r="E99" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F99" s="33">
+      <c r="F99" s="31">
         <v>0.1</v>
       </c>
-      <c r="G99" s="30" t="s">
+      <c r="G99" s="28" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C100" s="32" t="d">
+      <c r="C100" s="30" t="d">
         <v>2021-11-05</v>
       </c>
-      <c r="D100" s="30" t="s">
+      <c r="D100" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E100" s="30" t="s">
+      <c r="E100" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F100" s="33">
+      <c r="F100" s="31">
         <v>0.1</v>
       </c>
-      <c r="G100" s="30" t="s">
+      <c r="G100" s="28" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="101" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C101" s="32" t="d">
+      <c r="C101" s="30" t="d">
         <v>2021-11-05</v>
       </c>
-      <c r="D101" s="30" t="s">
+      <c r="D101" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E101" s="30" t="s">
+      <c r="E101" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F101" s="33">
+      <c r="F101" s="31">
         <v>0.1</v>
       </c>
-      <c r="G101" s="30" t="s">
+      <c r="G101" s="28" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="102" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C102" s="44" t="d">
+      <c r="C102" s="39" t="d">
         <v>2021-11-09</v>
       </c>
-      <c r="D102" s="30" t="s">
+      <c r="D102" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E102" s="30" t="s">
+      <c r="E102" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F102" s="45">
+      <c r="F102" s="40">
         <v>0.3</v>
       </c>
-      <c r="G102" s="30" t="s">
+      <c r="G102" s="28" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="103" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C103" s="44" t="d">
+      <c r="C103" s="39" t="d">
         <v>2021-11-10</v>
       </c>
-      <c r="D103" s="30" t="s">
+      <c r="D103" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="E103" s="30" t="s">
+      <c r="E103" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F103" s="45">
+      <c r="F103" s="40">
         <v>0.2</v>
       </c>
-      <c r="G103" s="30" t="s">
+      <c r="G103" s="28" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="104" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C104" s="44" t="d">
+      <c r="C104" s="39" t="d">
         <v>2021-11-10</v>
       </c>
-      <c r="D104" s="30" t="s">
+      <c r="D104" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E104" s="30" t="s">
+      <c r="E104" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F104" s="45">
+      <c r="F104" s="40">
         <v>0.2</v>
       </c>
-      <c r="G104" s="30" t="s">
+      <c r="G104" s="28" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="105" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C105" s="44" t="d">
+      <c r="C105" s="39" t="d">
         <v>2021-11-10</v>
       </c>
-      <c r="D105" s="30" t="s">
+      <c r="D105" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E105" s="30" t="s">
+      <c r="E105" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F105" s="45">
+      <c r="F105" s="40">
         <v>0.2</v>
       </c>
-      <c r="G105" s="30" t="s">
+      <c r="G105" s="28" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="106" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C106" s="44" t="d">
+      <c r="C106" s="39" t="d">
         <v>2021-11-10</v>
       </c>
-      <c r="D106" s="30" t="s">
+      <c r="D106" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E106" s="30" t="s">
+      <c r="E106" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F106" s="45">
+      <c r="F106" s="40">
         <v>0.2</v>
       </c>
-      <c r="G106" s="30" t="s">
+      <c r="G106" s="28" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="107" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C107" s="44" t="d">
+      <c r="C107" s="39" t="d">
         <v>2021-11-10</v>
       </c>
-      <c r="D107" s="30" t="s">
+      <c r="D107" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E107" s="30" t="s">
+      <c r="E107" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F107" s="45">
+      <c r="F107" s="40">
         <v>0.2</v>
       </c>
-      <c r="G107" s="30" t="s">
+      <c r="G107" s="28" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="108" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C108" s="46" t="d">
+      <c r="C108" s="41" t="d">
         <v>2021-11-10</v>
       </c>
-      <c r="D108" s="30" t="s">
+      <c r="D108" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="E108" s="30" t="s">
+      <c r="E108" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F108" s="45">
+      <c r="F108" s="40">
         <v>0.5</v>
       </c>
-      <c r="G108" s="30" t="s">
+      <c r="G108" s="28" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="109" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C109" s="46" t="d">
+      <c r="C109" s="41" t="d">
         <v>2021-11-10</v>
       </c>
-      <c r="D109" s="30" t="s">
+      <c r="D109" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E109" s="30" t="s">
+      <c r="E109" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F109" s="45">
+      <c r="F109" s="40">
         <v>0.4</v>
       </c>
-      <c r="G109" s="30" t="s">
+      <c r="G109" s="28" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="110" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C110" s="46" t="d">
+      <c r="C110" s="41" t="d">
         <v>2021-11-10</v>
       </c>
-      <c r="D110" s="30" t="s">
+      <c r="D110" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E110" s="30" t="s">
+      <c r="E110" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F110" s="45">
+      <c r="F110" s="40">
         <v>0.4</v>
       </c>
-      <c r="G110" s="30" t="s">
+      <c r="G110" s="28" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="111" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C111" s="46" t="d">
+      <c r="C111" s="41" t="d">
         <v>2021-11-10</v>
       </c>
-      <c r="D111" s="30" t="s">
+      <c r="D111" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E111" s="30" t="s">
+      <c r="E111" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F111" s="45">
+      <c r="F111" s="40">
         <v>0.4</v>
       </c>
-      <c r="G111" s="30" t="s">
+      <c r="G111" s="28" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="112" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C112" s="46" t="d">
+      <c r="C112" s="41" t="d">
         <v>2021-11-10</v>
       </c>
-      <c r="D112" s="30" t="s">
+      <c r="D112" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E112" s="30" t="s">
+      <c r="E112" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F112" s="45">
+      <c r="F112" s="40">
         <v>0.4</v>
       </c>
-      <c r="G112" s="30" t="s">
+      <c r="G112" s="28" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="113" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C113" s="46" t="d">
+      <c r="C113" s="41" t="d">
         <v>2021-11-10</v>
       </c>
-      <c r="D113" s="30" t="s">
+      <c r="D113" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E113" s="30" t="s">
+      <c r="E113" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F113" s="45">
+      <c r="F113" s="40">
         <v>0.8</v>
       </c>
-      <c r="G113" s="30" t="s">
+      <c r="G113" s="28" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="114" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C114" s="46" t="d">
+      <c r="C114" s="41" t="d">
         <v>2021-11-10</v>
       </c>
-      <c r="D114" s="30" t="s">
+      <c r="D114" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E114" s="30" t="s">
+      <c r="E114" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="F114" s="45">
+      <c r="F114" s="40">
         <v>0.3</v>
       </c>
-      <c r="G114" s="30" t="s">
+      <c r="G114" s="28" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="115" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C115" s="46" t="d">
+      <c r="C115" s="41" t="d">
         <v>2021-11-10</v>
       </c>
-      <c r="D115" s="30" t="s">
+      <c r="D115" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E115" s="30" t="s">
+      <c r="E115" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="F115" s="45">
+      <c r="F115" s="40">
         <v>0.3</v>
       </c>
-      <c r="G115" s="30" t="s">
+      <c r="G115" s="28" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="116" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C116" s="46" t="d">
+      <c r="C116" s="41" t="d">
         <v>2021-11-10</v>
       </c>
-      <c r="D116" s="30" t="s">
+      <c r="D116" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="E116" s="30" t="s">
+      <c r="E116" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F116" s="45">
+      <c r="F116" s="40">
         <v>0.8</v>
       </c>
-      <c r="G116" s="30" t="s">
+      <c r="G116" s="28" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="117" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C117" s="46" t="d">
+      <c r="C117" s="41" t="d">
         <v>2021-11-10</v>
       </c>
-      <c r="D117" s="30" t="s">
+      <c r="D117" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E117" s="30" t="s">
+      <c r="E117" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="F117" s="45">
+      <c r="F117" s="40">
         <v>0.9</v>
       </c>
-      <c r="G117" s="47" t="s">
+      <c r="G117" s="42" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="118" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C118" s="46" t="d">
+      <c r="C118" s="41" t="d">
         <v>2021-11-10</v>
       </c>
-      <c r="D118" s="30" t="s">
+      <c r="D118" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E118" s="30" t="s">
+      <c r="E118" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F118" s="45">
+      <c r="F118" s="40">
         <v>0.4</v>
       </c>
-      <c r="G118" s="30" t="s">
+      <c r="G118" s="28" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="119" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C119" s="46" t="d">
+      <c r="C119" s="41" t="d">
         <v>2021-11-10</v>
       </c>
-      <c r="D119" s="30" t="s">
+      <c r="D119" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E119" s="30" t="s">
+      <c r="E119" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F119" s="45">
+      <c r="F119" s="40">
         <v>0.4</v>
       </c>
-      <c r="G119" s="30" t="s">
+      <c r="G119" s="28" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="120" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C120" s="46" t="d">
+      <c r="C120" s="41" t="d">
         <v>2021-11-11</v>
       </c>
-      <c r="D120" s="30" t="s">
+      <c r="D120" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E120" s="30" t="s">
+      <c r="E120" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="F120" s="45">
+      <c r="F120" s="40">
         <v>0.3</v>
       </c>
-      <c r="G120" s="30" t="s">
+      <c r="G120" s="28" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="121" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C121" s="46" t="d">
+      <c r="C121" s="41" t="d">
         <v>2021-11-11</v>
       </c>
-      <c r="D121" s="30" t="s">
+      <c r="D121" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E121" s="30" t="s">
+      <c r="E121" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="F121" s="45">
+      <c r="F121" s="40">
         <v>0.3</v>
       </c>
-      <c r="G121" s="30" t="s">
+      <c r="G121" s="28" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="122" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C122" s="46" t="d">
+      <c r="C122" s="41" t="d">
         <v>2021-11-11</v>
       </c>
-      <c r="D122" s="30" t="s">
+      <c r="D122" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="E122" s="30" t="s">
+      <c r="E122" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F122" s="45">
+      <c r="F122" s="40">
         <v>1</v>
       </c>
-      <c r="G122" s="30" t="s">
+      <c r="G122" s="28" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="123" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C123" s="46" t="d">
+      <c r="C123" s="41" t="d">
         <v>2021-11-11</v>
       </c>
-      <c r="D123" s="30" t="s">
+      <c r="D123" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E123" s="30" t="s">
+      <c r="E123" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F123" s="45">
+      <c r="F123" s="40">
         <v>0.9</v>
       </c>
-      <c r="G123" s="30" t="s">
+      <c r="G123" s="28" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="124" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C124" s="46" t="d">
+      <c r="C124" s="41" t="d">
         <v>2021-11-11</v>
       </c>
-      <c r="D124" s="30" t="s">
+      <c r="D124" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E124" s="30" t="s">
+      <c r="E124" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F124" s="45">
+      <c r="F124" s="40">
         <v>1</v>
       </c>
-      <c r="G124" s="30" t="s">
+      <c r="G124" s="28" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="125" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C125" s="46" t="d">
+      <c r="C125" s="41" t="d">
         <v>2021-11-11</v>
       </c>
-      <c r="D125" s="47" t="s">
+      <c r="D125" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E125" s="47" t="s">
+      <c r="E125" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="F125" s="48">
+      <c r="F125" s="43">
         <v>0.5</v>
       </c>
-      <c r="G125" s="30" t="s">
+      <c r="G125" s="28" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="126" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C126" s="46" t="d">
+      <c r="C126" s="41" t="d">
         <v>2021-11-11</v>
       </c>
-      <c r="D126" s="30" t="s">
+      <c r="D126" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E126" s="30" t="s">
+      <c r="E126" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="F126" s="45">
+      <c r="F126" s="40">
         <v>1</v>
       </c>
-      <c r="G126" s="30" t="s">
+      <c r="G126" s="28" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="127" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C127" s="46" t="d">
+      <c r="C127" s="41" t="d">
         <v>2021-11-11</v>
       </c>
-      <c r="D127" s="30" t="s">
+      <c r="D127" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E127" s="30" t="s">
+      <c r="E127" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F127" s="45">
+      <c r="F127" s="40">
         <v>0.2</v>
       </c>
-      <c r="G127" s="30" t="s">
+      <c r="G127" s="28" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="128" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C128" s="41" t="d">
+      <c r="C128" s="39" t="d">
         <v>2021-11-17</v>
       </c>
-      <c r="D128" s="27" t="s">
+      <c r="D128" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E128" s="27" t="s">
+      <c r="E128" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F128" s="42">
+      <c r="F128" s="40">
         <v>0.3</v>
       </c>
-      <c r="G128" s="42" t="s">
+      <c r="G128" s="40" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="129" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C129" s="41" t="d">
+      <c r="C129" s="39" t="d">
         <v>2021-11-17</v>
       </c>
-      <c r="D129" s="27" t="s">
+      <c r="D129" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E129" s="27" t="s">
+      <c r="E129" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F129" s="42">
+      <c r="F129" s="40">
         <v>0.3</v>
       </c>
-      <c r="G129" s="42" t="s">
+      <c r="G129" s="40" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="130" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C130" s="41" t="d">
+      <c r="C130" s="39" t="d">
         <v>2021-11-17</v>
       </c>
-      <c r="D130" s="27" t="s">
+      <c r="D130" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="E130" s="27" t="s">
+      <c r="E130" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F130" s="42">
+      <c r="F130" s="40">
         <v>0.3</v>
       </c>
-      <c r="G130" s="42" t="s">
+      <c r="G130" s="40" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="131" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C131" s="41" t="d">
+      <c r="C131" s="39" t="d">
         <v>2021-11-17</v>
       </c>
-      <c r="D131" s="27" t="s">
+      <c r="D131" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E131" s="27" t="s">
+      <c r="E131" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F131" s="42">
+      <c r="F131" s="40">
         <v>0.3</v>
       </c>
-      <c r="G131" s="42" t="s">
+      <c r="G131" s="40" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="132" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C132" s="41" t="d">
+      <c r="C132" s="39" t="d">
         <v>2021-11-17</v>
       </c>
-      <c r="D132" s="27" t="s">
+      <c r="D132" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E132" s="27" t="s">
+      <c r="E132" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F132" s="42">
+      <c r="F132" s="40">
         <v>0.3</v>
       </c>
-      <c r="G132" s="42" t="s">
+      <c r="G132" s="40" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="133" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C133" s="41" t="d">
+      <c r="C133" s="39" t="d">
         <v>2021-11-17</v>
       </c>
-      <c r="D133" s="27" t="s">
+      <c r="D133" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="27" t="s">
+      <c r="E133" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="F133" s="42">
+      <c r="F133" s="40">
         <v>0.7</v>
       </c>
-      <c r="G133" s="42" t="s">
+      <c r="G133" s="40" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="134" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C134" s="41" t="d">
+      <c r="C134" s="39" t="d">
         <v>2021-11-17</v>
       </c>
-      <c r="D134" s="27" t="s">
+      <c r="D134" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E134" s="27" t="s">
+      <c r="E134" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="F134" s="42">
+      <c r="F134" s="40">
         <v>0.7</v>
       </c>
-      <c r="G134" s="42" t="s">
+      <c r="G134" s="40" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="135" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C135" s="41" t="d">
+      <c r="C135" s="39" t="d">
         <v>2021-11-17</v>
       </c>
-      <c r="D135" s="27" t="s">
+      <c r="D135" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="E135" s="27" t="s">
+      <c r="E135" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="F135" s="42">
+      <c r="F135" s="40">
         <v>0.7</v>
       </c>
-      <c r="G135" s="42" t="s">
+      <c r="G135" s="40" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="136" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C136" s="41" t="d">
+      <c r="C136" s="39" t="d">
         <v>2021-11-17</v>
       </c>
-      <c r="D136" s="27" t="s">
+      <c r="D136" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E136" s="27" t="s">
+      <c r="E136" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="F136" s="42">
+      <c r="F136" s="40">
         <v>0.7</v>
       </c>
-      <c r="G136" s="42" t="s">
+      <c r="G136" s="40" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="137" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C137" s="41" t="d">
+      <c r="C137" s="39" t="d">
         <v>2021-11-17</v>
       </c>
-      <c r="D137" s="27" t="s">
+      <c r="D137" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E137" s="27" t="s">
+      <c r="E137" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="F137" s="42">
+      <c r="F137" s="40">
         <v>0.7</v>
       </c>
-      <c r="G137" s="42" t="s">
+      <c r="G137" s="40" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="138" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C138" s="41" t="d">
+      <c r="C138" s="39" t="d">
         <v>2021-11-18</v>
       </c>
-      <c r="D138" s="27" t="s">
+      <c r="D138" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E138" s="27" t="s">
+      <c r="E138" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F138" s="42">
+      <c r="F138" s="40">
         <v>0.5</v>
       </c>
-      <c r="G138" s="42" t="s">
+      <c r="G138" s="40" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="139" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C139" s="41" t="d">
+      <c r="C139" s="39" t="d">
         <v>2021-11-18</v>
       </c>
-      <c r="D139" s="27" t="s">
+      <c r="D139" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="E139" s="27" t="s">
+      <c r="E139" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F139" s="42">
+      <c r="F139" s="40">
         <v>0.5</v>
       </c>
-      <c r="G139" s="42" t="s">
+      <c r="G139" s="40" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="140" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C140" s="41" t="d">
+      <c r="C140" s="39" t="d">
         <v>2021-11-18</v>
       </c>
-      <c r="D140" s="27" t="s">
+      <c r="D140" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E140" s="27" t="s">
+      <c r="E140" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F140" s="42">
+      <c r="F140" s="40">
         <v>0.5</v>
       </c>
-      <c r="G140" s="42" t="s">
+      <c r="G140" s="40" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="141" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C141" s="41" t="d">
+      <c r="C141" s="39" t="d">
         <v>2021-11-18</v>
       </c>
-      <c r="D141" s="27" t="s">
+      <c r="D141" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E141" s="27" t="s">
+      <c r="E141" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F141" s="42">
+      <c r="F141" s="40">
         <v>0.5</v>
       </c>
-      <c r="G141" s="42" t="s">
+      <c r="G141" s="40" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="142" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C142" s="41" t="d">
+      <c r="C142" s="39" t="d">
         <v>2021-11-18</v>
       </c>
-      <c r="D142" s="27" t="s">
+      <c r="D142" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E142" s="27" t="s">
+      <c r="E142" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="F142" s="42">
+      <c r="F142" s="40">
         <v>1</v>
       </c>
-      <c r="G142" s="42" t="s">
+      <c r="G142" s="40" t="s">
         <v>69</v>
       </c>
     </row>
@@ -4643,16 +4668,16 @@
       <c r="C143" s="39" t="d">
         <v>2021-11-19</v>
       </c>
-      <c r="D143" s="27" t="s">
+      <c r="D143" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E143" s="27" t="s">
+      <c r="E143" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F143" s="42">
+      <c r="F143" s="40">
         <v>1</v>
       </c>
-      <c r="G143" s="42" t="s">
+      <c r="G143" s="40" t="s">
         <v>66</v>
       </c>
     </row>
@@ -4660,16 +4685,16 @@
       <c r="C144" s="39" t="d">
         <v>2021-11-19</v>
       </c>
-      <c r="D144" s="27" t="s">
+      <c r="D144" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="E144" s="27" t="s">
+      <c r="E144" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F144" s="42">
+      <c r="F144" s="40">
         <v>1</v>
       </c>
-      <c r="G144" s="42" t="s">
+      <c r="G144" s="40" t="s">
         <v>66</v>
       </c>
     </row>
@@ -4677,16 +4702,16 @@
       <c r="C145" s="39" t="d">
         <v>2021-11-19</v>
       </c>
-      <c r="D145" s="27" t="s">
+      <c r="D145" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E145" s="27" t="s">
+      <c r="E145" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F145" s="24">
+      <c r="F145" s="40">
         <v>0.8</v>
       </c>
-      <c r="G145" s="42" t="s">
+      <c r="G145" s="40" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4694,16 +4719,16 @@
       <c r="C146" s="39" t="d">
         <v>2021-11-19</v>
       </c>
-      <c r="D146" s="27" t="s">
+      <c r="D146" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E146" s="27" t="s">
+      <c r="E146" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F146" s="24">
+      <c r="F146" s="40">
         <v>1</v>
       </c>
-      <c r="G146" s="42" t="s">
+      <c r="G146" s="40" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4711,16 +4736,16 @@
       <c r="C147" s="39" t="d">
         <v>2021-11-19</v>
       </c>
-      <c r="D147" s="27" t="s">
+      <c r="D147" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E147" s="27" t="s">
+      <c r="E147" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F147" s="24">
+      <c r="F147" s="40">
         <v>0.1</v>
       </c>
-      <c r="G147" s="42" t="s">
+      <c r="G147" s="40" t="s">
         <v>48</v>
       </c>
     </row>
@@ -4728,16 +4753,16 @@
       <c r="C148" s="39" t="d">
         <v>2021-11-19</v>
       </c>
-      <c r="D148" s="27" t="s">
+      <c r="D148" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E148" s="27" t="s">
+      <c r="E148" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F148" s="24">
+      <c r="F148" s="40">
         <v>0.1</v>
       </c>
-      <c r="G148" s="42" t="s">
+      <c r="G148" s="40" t="s">
         <v>71</v>
       </c>
     </row>
@@ -4745,320 +4770,599 @@
       <c r="C149" s="39" t="d">
         <v>2021-11-19</v>
       </c>
-      <c r="D149" s="27" t="s">
+      <c r="D149" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E149" s="24" t="s">
+      <c r="E149" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="F149" s="24">
+      <c r="F149" s="40">
         <v>0.5</v>
       </c>
-      <c r="G149" s="42" t="s">
+      <c r="G149" s="40" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="150" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C150" s="50"/>
-      <c r="G150" s="49"/>
+      <c r="C150" s="46" t="d">
+        <v>2021-11-24</v>
+      </c>
+      <c r="D150" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="E150" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="F150" s="49">
+        <v>0.3</v>
+      </c>
+      <c r="G150" s="49" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="151" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C151" s="1"/>
-      <c r="G151" s="49"/>
+      <c r="C151" s="46" t="d">
+        <v>2021-11-24</v>
+      </c>
+      <c r="D151" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="E151" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="F151" s="49">
+        <v>0.3</v>
+      </c>
+      <c r="G151" s="49" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="152" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C152" s="1"/>
-      <c r="G152" s="49"/>
+      <c r="C152" s="46" t="d">
+        <v>2021-11-24</v>
+      </c>
+      <c r="D152" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="E152" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="F152" s="49">
+        <v>0.3</v>
+      </c>
+      <c r="G152" s="49" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="153" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C153" s="1"/>
-      <c r="G153" s="49"/>
+      <c r="C153" s="46" t="d">
+        <v>2021-11-24</v>
+      </c>
+      <c r="D153" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E153" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="F153" s="49">
+        <v>0.3</v>
+      </c>
+      <c r="G153" s="49" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="154" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C154" s="1"/>
-      <c r="G154" s="49"/>
+      <c r="C154" s="46" t="d">
+        <v>2021-11-24</v>
+      </c>
+      <c r="D154" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="E154" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="F154" s="49">
+        <v>0.3</v>
+      </c>
+      <c r="G154" s="49" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="155" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C155" s="1"/>
-      <c r="G155" s="49"/>
+      <c r="C155" s="46" t="d">
+        <v>2021-11-24</v>
+      </c>
+      <c r="D155" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="E155" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="F155" s="49">
+        <v>0.7</v>
+      </c>
+      <c r="G155" s="49" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="156" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C156" s="1"/>
-      <c r="G156" s="49"/>
+      <c r="C156" s="46" t="d">
+        <v>2021-11-24</v>
+      </c>
+      <c r="D156" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="E156" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="F156" s="49">
+        <v>0.7</v>
+      </c>
+      <c r="G156" s="49" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="157" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C157" s="1"/>
-      <c r="G157" s="49"/>
+      <c r="C157" s="50" t="d">
+        <v>2021-11-24</v>
+      </c>
+      <c r="D157" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="E157" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="F157" s="51">
+        <v>0.7</v>
+      </c>
+      <c r="G157" s="49" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="158" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C158" s="1"/>
-      <c r="G158" s="49"/>
+      <c r="C158" s="50" t="d">
+        <v>2021-11-24</v>
+      </c>
+      <c r="D158" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E158" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="F158" s="51">
+        <v>0.7</v>
+      </c>
+      <c r="G158" s="49" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="159" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C159" s="1"/>
-      <c r="G159" s="49"/>
+      <c r="C159" s="50" t="d">
+        <v>2021-11-24</v>
+      </c>
+      <c r="D159" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="E159" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="F159" s="51">
+        <v>0.7</v>
+      </c>
+      <c r="G159" s="49" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="160" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C160" s="1"/>
-      <c r="G160" s="49"/>
+      <c r="C160" s="50" t="d">
+        <v>2021-11-25</v>
+      </c>
+      <c r="D160" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="E160" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="F160" s="51">
+        <v>1</v>
+      </c>
+      <c r="G160" s="49" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="161" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C161" s="1"/>
-      <c r="G161" s="49"/>
+      <c r="C161" s="50" t="d">
+        <v>2021-11-25</v>
+      </c>
+      <c r="D161" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="E161" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="F161" s="52">
+        <v>1</v>
+      </c>
+      <c r="G161" s="49" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="162" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C162" s="1"/>
-      <c r="G162" s="49"/>
+      <c r="C162" s="50" t="d">
+        <v>2021-11-25</v>
+      </c>
+      <c r="D162" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E162" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="F162" s="51">
+        <v>1</v>
+      </c>
+      <c r="G162" s="49" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="163" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C163" s="1"/>
-      <c r="G163" s="49"/>
+      <c r="C163" s="50" t="d">
+        <v>2021-11-25</v>
+      </c>
+      <c r="D163" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="E163" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="F163" s="51">
+        <v>1</v>
+      </c>
+      <c r="G163" s="49" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="164" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C164" s="1"/>
-      <c r="G164" s="49"/>
+      <c r="C164" s="50" t="d">
+        <v>2021-11-25</v>
+      </c>
+      <c r="D164" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="E164" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="F164" s="51">
+        <v>0.5</v>
+      </c>
+      <c r="G164" s="49" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="165" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C165" s="1"/>
-      <c r="G165" s="49"/>
+      <c r="C165" s="50" t="d">
+        <v>2021-11-26</v>
+      </c>
+      <c r="D165" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="E165" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="F165" s="51">
+        <v>0.5</v>
+      </c>
+      <c r="G165" s="49" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="166" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C166" s="1"/>
-      <c r="G166" s="49"/>
+      <c r="C166" s="50" t="d">
+        <v>2021-11-26</v>
+      </c>
+      <c r="D166" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E166" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="F166" s="51">
+        <v>0.5</v>
+      </c>
+      <c r="G166" s="49" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="167" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C167" s="1"/>
-      <c r="G167" s="49"/>
+      <c r="C167" s="50" t="d">
+        <v>2021-11-26</v>
+      </c>
+      <c r="D167" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="E167" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="F167" s="51">
+        <v>0.5</v>
+      </c>
+      <c r="G167" s="49" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="168" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C168" s="1"/>
-      <c r="G168" s="49"/>
+      <c r="C168" s="50" t="d">
+        <v>2021-11-26</v>
+      </c>
+      <c r="D168" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="E168" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="F168" s="51">
+        <v>0.3</v>
+      </c>
+      <c r="G168" s="49" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="169" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C169" s="1"/>
-      <c r="G169" s="49"/>
+      <c r="C169" s="50" t="d">
+        <v>2021-11-26</v>
+      </c>
+      <c r="D169" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="E169" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="F169" s="51">
+        <v>0.8</v>
+      </c>
+      <c r="G169" s="49" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="170" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C170" s="1"/>
-      <c r="G170" s="49"/>
+      <c r="C170" s="50" t="d">
+        <v>2021-11-26</v>
+      </c>
+      <c r="D170" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="E170" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F170" s="51">
+        <v>0.2</v>
+      </c>
+      <c r="G170" s="49" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="171" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C171" s="1"/>
-      <c r="G171" s="49"/>
-    </row>
-    <row r="172" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C172" s="1"/>
-      <c r="G172" s="49"/>
+      <c r="C171" s="50" t="d">
+        <v>2021-11-26</v>
+      </c>
+      <c r="D171" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="E171" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F171" s="51">
+        <v>0.2</v>
+      </c>
+      <c r="G171" s="49" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="173" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C173" s="1"/>
-      <c r="G173" s="49"/>
+      <c r="C173" s="44"/>
+      <c r="D173" s="45"/>
+      <c r="E173" s="45"/>
+      <c r="F173" s="44"/>
+      <c r="G173" s="44"/>
     </row>
     <row r="174" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C174" s="1"/>
-      <c r="G174" s="49"/>
+      <c r="C174" s="44"/>
+      <c r="D174" s="45"/>
+      <c r="E174" s="45"/>
+      <c r="F174" s="44"/>
+      <c r="G174" s="44"/>
     </row>
     <row r="175" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C175" s="1"/>
-      <c r="G175" s="49"/>
+      <c r="C175" s="44"/>
+      <c r="D175" s="45"/>
+      <c r="E175" s="45"/>
+      <c r="F175" s="44"/>
+      <c r="G175" s="44"/>
     </row>
     <row r="176" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C176" s="1"/>
-      <c r="G176" s="49"/>
-    </row>
-    <row r="177" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C177" s="1"/>
-      <c r="G177" s="49"/>
-    </row>
-    <row r="178" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C178" s="1"/>
-      <c r="G178" s="49"/>
-    </row>
-    <row r="179" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C179" s="1"/>
-      <c r="G179" s="49"/>
+      <c r="G176" s="44"/>
     </row>
     <row r="180" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C180" s="1"/>
-      <c r="G180" s="49"/>
+      <c r="G180" s="44"/>
     </row>
     <row r="181" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C181" s="1"/>
-      <c r="G181" s="49"/>
+      <c r="G181" s="44"/>
     </row>
     <row r="182" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C182" s="1"/>
-      <c r="G182" s="49"/>
+      <c r="G182" s="44"/>
     </row>
     <row r="183" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C183" s="1"/>
-      <c r="G183" s="49"/>
+      <c r="G183" s="44"/>
     </row>
     <row r="184" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C184" s="1"/>
-      <c r="G184" s="49"/>
+      <c r="G184" s="44"/>
     </row>
     <row r="185" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C185" s="1"/>
-      <c r="G185" s="49"/>
+      <c r="G185" s="44"/>
     </row>
     <row r="186" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C186" s="1"/>
-      <c r="G186" s="49"/>
+      <c r="G186" s="44"/>
     </row>
     <row r="187" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C187" s="1"/>
-      <c r="G187" s="49"/>
+      <c r="G187" s="44"/>
     </row>
     <row r="188" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C188" s="1"/>
-      <c r="G188" s="49"/>
+      <c r="G188" s="44"/>
     </row>
     <row r="189" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C189" s="1"/>
-      <c r="G189" s="49"/>
+      <c r="G189" s="44"/>
     </row>
     <row r="190" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C190" s="1"/>
-      <c r="G190" s="49"/>
+      <c r="G190" s="44"/>
     </row>
     <row r="191" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C191" s="1"/>
-      <c r="G191" s="49"/>
+      <c r="G191" s="44"/>
     </row>
     <row r="192" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C192" s="1"/>
-      <c r="G192" s="49"/>
+      <c r="G192" s="44"/>
     </row>
     <row r="193" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C193" s="1"/>
-      <c r="G193" s="49"/>
+      <c r="G193" s="44"/>
     </row>
     <row r="194" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C194" s="1"/>
-      <c r="G194" s="49"/>
+      <c r="G194" s="44"/>
     </row>
     <row r="195" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C195" s="1"/>
-      <c r="G195" s="49"/>
+      <c r="G195" s="44"/>
     </row>
     <row r="196" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C196" s="1"/>
-      <c r="G196" s="49"/>
+      <c r="G196" s="44"/>
     </row>
     <row r="197" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C197" s="1"/>
-      <c r="G197" s="49"/>
+      <c r="G197" s="44"/>
     </row>
     <row r="198" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C198" s="1"/>
-      <c r="G198" s="49"/>
+      <c r="G198" s="44"/>
     </row>
     <row r="199" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C199" s="1"/>
-      <c r="G199" s="49"/>
+      <c r="G199" s="44"/>
     </row>
     <row r="200" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C200" s="1"/>
-      <c r="G200" s="49"/>
+      <c r="G200" s="44"/>
     </row>
     <row r="201" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C201" s="1"/>
-      <c r="G201" s="49"/>
+      <c r="G201" s="44"/>
     </row>
     <row r="202" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C202" s="1"/>
-      <c r="G202" s="49"/>
+      <c r="G202" s="44"/>
     </row>
     <row r="203" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C203" s="1"/>
-      <c r="G203" s="49"/>
+      <c r="G203" s="44"/>
     </row>
     <row r="204" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C204" s="1"/>
-      <c r="G204" s="49"/>
+      <c r="G204" s="44"/>
     </row>
     <row r="205" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C205" s="1"/>
-      <c r="G205" s="49"/>
+      <c r="G205" s="44"/>
     </row>
     <row r="206" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C206" s="1"/>
-      <c r="G206" s="49"/>
+      <c r="G206" s="44"/>
     </row>
     <row r="207" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C207" s="1"/>
-      <c r="G207" s="49"/>
+      <c r="G207" s="44"/>
     </row>
     <row r="208" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C208" s="1"/>
-      <c r="G208" s="49"/>
+      <c r="G208" s="44"/>
     </row>
     <row r="209" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C209" s="1"/>
-      <c r="G209" s="49"/>
+      <c r="G209" s="44"/>
     </row>
     <row r="210" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C210" s="1"/>
-      <c r="G210" s="49"/>
+      <c r="G210" s="44"/>
     </row>
     <row r="211" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C211" s="1"/>
-      <c r="G211" s="49"/>
+      <c r="G211" s="44"/>
     </row>
     <row r="212" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C212" s="1"/>
-      <c r="G212" s="49"/>
+      <c r="G212" s="44"/>
     </row>
     <row r="213" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C213" s="1"/>
-      <c r="G213" s="49"/>
+      <c r="G213" s="44"/>
     </row>
     <row r="214" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C214" s="1"/>
-      <c r="G214" s="49"/>
+      <c r="G214" s="44"/>
     </row>
     <row r="215" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C215" s="1"/>
-      <c r="G215" s="49"/>
+      <c r="G215" s="44"/>
     </row>
     <row r="216" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C216" s="1"/>
-      <c r="G216" s="49"/>
+      <c r="G216" s="44"/>
     </row>
     <row r="217" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C217" s="1"/>
-      <c r="G217" s="49"/>
+      <c r="G217" s="44"/>
     </row>
     <row r="218" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C218" s="1"/>
-      <c r="G218" s="49"/>
+      <c r="G218" s="44"/>
     </row>
     <row r="219" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C219" s="1"/>
-      <c r="G219" s="49"/>
+      <c r="G219" s="44"/>
     </row>
     <row r="220" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C220" s="1"/>
-      <c r="G220" s="49"/>
+      <c r="G220" s="44"/>
     </row>
     <row r="221" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C221" s="40"/>
+      <c r="C221" s="37"/>
     </row>
     <row r="222" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C222" s="40"/>
+      <c r="C222" s="37"/>
     </row>
     <row r="223" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C223" s="40"/>
+      <c r="C223" s="37"/>
     </row>
     <row r="224" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C224" s="40"/>
+      <c r="C224" s="37"/>
     </row>
     <row r="225" spans="3:3" x14ac:dyDescent="0.15">
-      <c r="C225" s="40"/>
+      <c r="C225" s="37"/>
     </row>
     <row r="226" spans="3:3" x14ac:dyDescent="0.15">
-      <c r="C226" s="40"/>
+      <c r="C226" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39370078740157505" bottom="0.39370078740157505" header="0" footer="0"/>
@@ -5072,10 +5376,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -5090,10 +5394,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>47</v>
       </c>
     </row>
@@ -5162,13 +5466,15 @@
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="16">
-        <v>0.1</v>
-      </c>
-      <c r="D6" s="16"/>
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0.2</v>
+      </c>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
       <c r="G6" s="17">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
@@ -5176,95 +5482,67 @@
         <v>21</v>
       </c>
       <c r="B7" s="15">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="C7" s="16">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="D7" s="16">
-        <v>1.5</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
+        <v>1</v>
+      </c>
+      <c r="E7" s="16">
+        <v>1</v>
+      </c>
+      <c r="F7" s="16">
+        <v>1</v>
+      </c>
       <c r="G7" s="17">
-        <v>3.1</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="15">
+        <v>1.2</v>
+      </c>
       <c r="C8" s="16">
-        <v>1.3</v>
-      </c>
-      <c r="D8" s="16"/>
+        <v>1.2</v>
+      </c>
+      <c r="D8" s="16">
+        <v>1</v>
+      </c>
       <c r="E8" s="16">
-        <v>1.5</v>
-      </c>
-      <c r="F8" s="16"/>
+        <v>1.2</v>
+      </c>
+      <c r="F8" s="16">
+        <v>1.2</v>
+      </c>
       <c r="G8" s="17">
-        <v>2.8</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="15">
-        <v>0.7</v>
-      </c>
-      <c r="C9" s="16">
-        <v>0.7</v>
-      </c>
-      <c r="D9" s="16">
-        <v>0.7</v>
-      </c>
-      <c r="E9" s="16">
-        <v>0.7</v>
-      </c>
-      <c r="F9" s="16">
-        <v>0.7</v>
-      </c>
-      <c r="G9" s="17">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16">
-        <v>1.5</v>
-      </c>
-      <c r="G10" s="17">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="18" t="s">
+      <c r="A9" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B9" s="19">
         <v>2.5</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C9" s="20">
         <v>2.5</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D9" s="20">
         <v>2.5</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E9" s="20">
         <v>2.5</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F9" s="20">
         <v>2.5</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G9" s="21">
         <v>12.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new workbook + updated project tracking
</commit_message>
<xml_diff>
--- a/project_management/project_tracking_gnlg2.xlsx
+++ b/project_management/project_tracking_gnlg2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivo/repositories/GNLG2/project_management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5756B8B9-8C8A-8C47-B121-1BAB590B5C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B15C93E8-A941-BA45-B455-F3B8C8610AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tab" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="70" r:id="rId3"/>
+    <pivotCache cacheId="36" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="469" uniqueCount="77">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="536" uniqueCount="81">
   <si>
     <t>CM</t>
   </si>
@@ -260,6 +260,18 @@
   </si>
   <si>
     <t>Laravel development</t>
+  </si>
+  <si>
+    <t>Working IRL</t>
+  </si>
+  <si>
+    <t>Occupied by intership applications</t>
+  </si>
+  <si>
+    <t>Occupied by urgent projects</t>
+  </si>
+  <si>
+    <t>Project Tracking finishing touches</t>
   </si>
 </sst>
 </file>
@@ -673,7 +685,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -759,26 +771,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -823,13 +843,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDateIso="2021-11-26T16:52:48.529999698512255850" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="188" xr:uid="{33C243A7-C20F-9A41-84D4-AFCEDFA037F4}">
+<pivotCacheDefinition xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDateIso="2021-12-05T15:41:56.29999999422579900" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="188" xr:uid="{33C243A7-C20F-9A41-84D4-AFCEDFA037F4}">
   <cacheSource type="worksheet">
     <worksheetSource ref="C34:G222" sheet="Tab"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2021-10-22T00:00:00" maxDate="2021-11-27T00:00:00" count="19">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2021-10-22T00:00:00" maxDate="2021-12-06T00:00:00" count="23">
         <d v="2021-10-22T00:00:00"/>
         <d v="2021-10-27T00:00:00"/>
         <d v="2021-10-28T00:00:00"/>
@@ -848,6 +868,10 @@
         <d v="2021-11-24T00:00:00"/>
         <d v="2021-11-25T00:00:00"/>
         <d v="2021-11-26T00:00:00"/>
+        <d v="2021-11-28T00:00:00"/>
+        <d v="2021-12-01T00:00:00"/>
+        <d v="2021-12-03T00:00:00"/>
+        <d v="2021-12-05T00:00:00"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -1854,370 +1878,370 @@
   </r>
   <r>
     <x v="18"/>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="0.5"/>
+    <s v="Laravel development"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="0.5"/>
+    <s v="Laravel development"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.5"/>
+    <s v="Laravel development"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="0.5"/>
+    <s v="Laravel development"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="0.4"/>
+    <s v="Laravel development"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="0.7"/>
+    <s v="Update the team on laravel project + development"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="0.7"/>
+    <s v="Update the team on laravel project + development"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="0.7"/>
+    <s v="Update the team on laravel project + development"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.7"/>
+    <s v="Update the team on laravel project + development"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="0.7"/>
+    <s v="Update the team on laravel project + development"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.3"/>
+    <s v="Metting with M. Oudot"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="0.3"/>
+    <s v="Occupied by IRL complications"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="0.3"/>
+    <s v="Working IRL"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="0.3"/>
+    <s v="Occupied by intership applications"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="0.3"/>
+    <s v="Occupied by intership applications"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1"/>
+    <s v="Workbook redaction"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1"/>
+    <s v="Workbook redaction"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1"/>
+    <s v="Workbook redaction"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1"/>
+    <s v="Workbook redaction"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <x v="3"/>
+    <x v="8"/>
+    <n v="0.9"/>
+    <s v="Occupied by urgent projects"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="0.1"/>
+    <s v="Project Tracking"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.1"/>
+    <s v="Project Tracking finishing touches"/>
+  </r>
+  <r>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="18"/>
+    <x v="22"/>
     <x v="5"/>
     <x v="9"/>
     <m/>
     <m/>
   </r>
-  <r>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{56ABA1B9-0D18-E44D-8AA9-6D65D511342F}" name="DataPilot1" cacheId="70" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" enableDrill="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" compact="0" compactData="0">
-  <location ref="A3:G9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{56ABA1B9-0D18-E44D-8AA9-6D65D511342F}" name="DataPilot1" cacheId="36" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" enableDrill="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" compact="0" compactData="0">
+  <location ref="A3:G10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="5">
     <pivotField axis="axisPage" compact="0" outline="0" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="20">
+      <items count="24">
         <item h="1" x="0"/>
         <item h="1" x="1"/>
         <item h="1" x="2"/>
@@ -2226,7 +2250,7 @@
         <item h="1" x="6"/>
         <item h="1" x="7"/>
         <item h="1" x="8"/>
-        <item h="1" x="18"/>
+        <item h="1" x="22"/>
         <item h="1" x="5"/>
         <item h="1" x="10"/>
         <item h="1" x="11"/>
@@ -2234,9 +2258,13 @@
         <item h="1" x="12"/>
         <item h="1" x="13"/>
         <item h="1" x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
+        <item h="1" x="15"/>
+        <item h="1" x="16"/>
+        <item h="1" x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2271,7 +2299,7 @@
   <rowFields count="1">
     <field x="2"/>
   </rowFields>
-  <rowItems count="5">
+  <rowItems count="6">
     <i>
       <x/>
     </i>
@@ -2283,6 +2311,9 @@
     </i>
     <i>
       <x v="5"/>
+    </i>
+    <i>
+      <x v="9"/>
     </i>
     <i t="grand">
       <x/>
@@ -2625,8 +2656,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="E166" sqref="E166"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="F185" sqref="F185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -4784,13 +4815,13 @@
       </c>
     </row>
     <row r="150" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C150" s="46" t="d">
+      <c r="C150" s="48" t="d">
         <v>2021-11-24</v>
       </c>
-      <c r="D150" s="47" t="s">
+      <c r="D150" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E150" s="48" t="s">
+      <c r="E150" s="28" t="s">
         <v>19</v>
       </c>
       <c r="F150" s="49">
@@ -4801,13 +4832,13 @@
       </c>
     </row>
     <row r="151" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C151" s="46" t="d">
+      <c r="C151" s="48" t="d">
         <v>2021-11-24</v>
       </c>
-      <c r="D151" s="47" t="s">
+      <c r="D151" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="E151" s="47" t="s">
+      <c r="E151" s="28" t="s">
         <v>19</v>
       </c>
       <c r="F151" s="49">
@@ -4818,13 +4849,13 @@
       </c>
     </row>
     <row r="152" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C152" s="46" t="d">
+      <c r="C152" s="48" t="d">
         <v>2021-11-24</v>
       </c>
-      <c r="D152" s="47" t="s">
+      <c r="D152" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E152" s="47" t="s">
+      <c r="E152" s="28" t="s">
         <v>19</v>
       </c>
       <c r="F152" s="49">
@@ -4835,13 +4866,13 @@
       </c>
     </row>
     <row r="153" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C153" s="46" t="d">
+      <c r="C153" s="48" t="d">
         <v>2021-11-24</v>
       </c>
-      <c r="D153" s="47" t="s">
+      <c r="D153" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E153" s="47" t="s">
+      <c r="E153" s="28" t="s">
         <v>19</v>
       </c>
       <c r="F153" s="49">
@@ -4852,13 +4883,13 @@
       </c>
     </row>
     <row r="154" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C154" s="46" t="d">
+      <c r="C154" s="48" t="d">
         <v>2021-11-24</v>
       </c>
-      <c r="D154" s="47" t="s">
+      <c r="D154" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E154" s="47" t="s">
+      <c r="E154" s="28" t="s">
         <v>19</v>
       </c>
       <c r="F154" s="49">
@@ -4869,13 +4900,13 @@
       </c>
     </row>
     <row r="155" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C155" s="46" t="d">
+      <c r="C155" s="48" t="d">
         <v>2021-11-24</v>
       </c>
-      <c r="D155" s="47" t="s">
+      <c r="D155" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E155" s="47" t="s">
+      <c r="E155" s="28" t="s">
         <v>13</v>
       </c>
       <c r="F155" s="49">
@@ -4886,13 +4917,13 @@
       </c>
     </row>
     <row r="156" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C156" s="46" t="d">
+      <c r="C156" s="48" t="d">
         <v>2021-11-24</v>
       </c>
-      <c r="D156" s="47" t="s">
+      <c r="D156" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="E156" s="47" t="s">
+      <c r="E156" s="28" t="s">
         <v>13</v>
       </c>
       <c r="F156" s="49">
@@ -4906,10 +4937,10 @@
       <c r="C157" s="50" t="d">
         <v>2021-11-24</v>
       </c>
-      <c r="D157" s="47" t="s">
+      <c r="D157" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E157" s="47" t="s">
+      <c r="E157" s="28" t="s">
         <v>13</v>
       </c>
       <c r="F157" s="51">
@@ -4923,10 +4954,10 @@
       <c r="C158" s="50" t="d">
         <v>2021-11-24</v>
       </c>
-      <c r="D158" s="47" t="s">
+      <c r="D158" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E158" s="47" t="s">
+      <c r="E158" s="28" t="s">
         <v>13</v>
       </c>
       <c r="F158" s="51">
@@ -4940,10 +4971,10 @@
       <c r="C159" s="50" t="d">
         <v>2021-11-24</v>
       </c>
-      <c r="D159" s="47" t="s">
+      <c r="D159" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E159" s="47" t="s">
+      <c r="E159" s="28" t="s">
         <v>13</v>
       </c>
       <c r="F159" s="51">
@@ -4957,7 +4988,7 @@
       <c r="C160" s="50" t="d">
         <v>2021-11-25</v>
       </c>
-      <c r="D160" s="47" t="s">
+      <c r="D160" s="28" t="s">
         <v>8</v>
       </c>
       <c r="E160" s="51" t="s">
@@ -4974,13 +5005,13 @@
       <c r="C161" s="50" t="d">
         <v>2021-11-25</v>
       </c>
-      <c r="D161" s="47" t="s">
+      <c r="D161" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E161" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="F161" s="52">
+      <c r="F161" s="49">
         <v>1</v>
       </c>
       <c r="G161" s="49" t="s">
@@ -4991,7 +5022,7 @@
       <c r="C162" s="50" t="d">
         <v>2021-11-25</v>
       </c>
-      <c r="D162" s="47" t="s">
+      <c r="D162" s="28" t="s">
         <v>4</v>
       </c>
       <c r="E162" s="51" t="s">
@@ -5008,7 +5039,7 @@
       <c r="C163" s="50" t="d">
         <v>2021-11-25</v>
       </c>
-      <c r="D163" s="47" t="s">
+      <c r="D163" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E163" s="51" t="s">
@@ -5042,7 +5073,7 @@
       <c r="C165" s="50" t="d">
         <v>2021-11-26</v>
       </c>
-      <c r="D165" s="47" t="s">
+      <c r="D165" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E165" s="51" t="s">
@@ -5059,7 +5090,7 @@
       <c r="C166" s="50" t="d">
         <v>2021-11-26</v>
       </c>
-      <c r="D166" s="47" t="s">
+      <c r="D166" s="28" t="s">
         <v>4</v>
       </c>
       <c r="E166" s="51" t="s">
@@ -5076,7 +5107,7 @@
       <c r="C167" s="50" t="d">
         <v>2021-11-26</v>
       </c>
-      <c r="D167" s="47" t="s">
+      <c r="D167" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E167" s="51" t="s">
@@ -5093,7 +5124,7 @@
       <c r="C168" s="50" t="d">
         <v>2021-11-26</v>
       </c>
-      <c r="D168" s="47" t="s">
+      <c r="D168" s="28" t="s">
         <v>8</v>
       </c>
       <c r="E168" s="51" t="s">
@@ -5157,102 +5188,379 @@
         <v>73</v>
       </c>
     </row>
+    <row r="172" spans="3:7" x14ac:dyDescent="0.15">
+      <c r="C172" s="52" t="d">
+        <v>2021-11-28</v>
+      </c>
+      <c r="D172" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="E172" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="F172" s="53">
+        <v>0.5</v>
+      </c>
+      <c r="G172" s="47" t="s">
+        <v>76</v>
+      </c>
+    </row>
     <row r="173" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C173" s="44"/>
-      <c r="D173" s="45"/>
-      <c r="E173" s="45"/>
-      <c r="F173" s="44"/>
-      <c r="G173" s="44"/>
+      <c r="C173" s="52" t="d">
+        <v>2021-11-28</v>
+      </c>
+      <c r="D173" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="E173" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="F173" s="53">
+        <v>0.5</v>
+      </c>
+      <c r="G173" s="47" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="174" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C174" s="44"/>
-      <c r="D174" s="45"/>
-      <c r="E174" s="45"/>
-      <c r="F174" s="44"/>
-      <c r="G174" s="44"/>
+      <c r="C174" s="52" t="d">
+        <v>2021-11-28</v>
+      </c>
+      <c r="D174" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="E174" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="F174" s="53">
+        <v>0.5</v>
+      </c>
+      <c r="G174" s="47" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="175" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C175" s="44"/>
-      <c r="D175" s="45"/>
-      <c r="E175" s="45"/>
-      <c r="F175" s="44"/>
-      <c r="G175" s="44"/>
+      <c r="C175" s="52" t="d">
+        <v>2021-11-28</v>
+      </c>
+      <c r="D175" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E175" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="F175" s="53">
+        <v>0.5</v>
+      </c>
+      <c r="G175" s="47" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="176" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C176" s="1"/>
-      <c r="G176" s="44"/>
+      <c r="C176" s="52" t="d">
+        <v>2021-11-28</v>
+      </c>
+      <c r="D176" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E176" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="F176" s="53">
+        <v>0.4</v>
+      </c>
+      <c r="G176" s="47" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="177" spans="3:7" x14ac:dyDescent="0.15">
+      <c r="C177" s="54" t="d">
+        <v>2021-12-01</v>
+      </c>
+      <c r="D177" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="E177" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="F177" s="47">
+        <v>0.7</v>
+      </c>
+      <c r="G177" s="47" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="178" spans="3:7" x14ac:dyDescent="0.15">
+      <c r="C178" s="54" t="d">
+        <v>2021-12-01</v>
+      </c>
+      <c r="D178" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E178" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="F178" s="47">
+        <v>0.7</v>
+      </c>
+      <c r="G178" s="47" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="179" spans="3:7" x14ac:dyDescent="0.15">
+      <c r="C179" s="54" t="d">
+        <v>2021-12-01</v>
+      </c>
+      <c r="D179" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="E179" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="F179" s="53">
+        <v>0.7</v>
+      </c>
+      <c r="G179" s="47" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="180" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C180" s="1"/>
-      <c r="G180" s="44"/>
+      <c r="C180" s="54" t="d">
+        <v>2021-12-01</v>
+      </c>
+      <c r="D180" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="E180" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="F180" s="53">
+        <v>0.7</v>
+      </c>
+      <c r="G180" s="47" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="181" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C181" s="1"/>
-      <c r="G181" s="44"/>
+      <c r="C181" s="54" t="d">
+        <v>2021-12-01</v>
+      </c>
+      <c r="D181" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E181" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="F181" s="53">
+        <v>0.7</v>
+      </c>
+      <c r="G181" s="47" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="182" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C182" s="1"/>
-      <c r="G182" s="44"/>
+      <c r="C182" s="52" t="d">
+        <v>2021-12-03</v>
+      </c>
+      <c r="D182" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="E182" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F182" s="47">
+        <v>0.3</v>
+      </c>
+      <c r="G182" s="47" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="183" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C183" s="1"/>
-      <c r="G183" s="44"/>
+      <c r="C183" s="52" t="d">
+        <v>2021-12-03</v>
+      </c>
+      <c r="D183" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="E183" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F183" s="47">
+        <v>0.3</v>
+      </c>
+      <c r="G183" s="47" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="184" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C184" s="1"/>
-      <c r="G184" s="44"/>
+      <c r="C184" s="52" t="d">
+        <v>2021-12-03</v>
+      </c>
+      <c r="D184" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E184" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F184" s="47">
+        <v>0.3</v>
+      </c>
+      <c r="G184" s="47" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="185" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C185" s="1"/>
-      <c r="G185" s="44"/>
+      <c r="C185" s="52" t="d">
+        <v>2021-12-03</v>
+      </c>
+      <c r="D185" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="E185" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F185" s="47">
+        <v>0.3</v>
+      </c>
+      <c r="G185" s="47" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="186" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C186" s="1"/>
-      <c r="G186" s="44"/>
+      <c r="C186" s="52" t="d">
+        <v>2021-12-03</v>
+      </c>
+      <c r="D186" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E186" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F186" s="47">
+        <v>0.3</v>
+      </c>
+      <c r="G186" s="47" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="187" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C187" s="1"/>
-      <c r="G187" s="44"/>
+      <c r="C187" s="52" t="d">
+        <v>2021-12-05</v>
+      </c>
+      <c r="D187" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E187" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="F187" s="53">
+        <v>1</v>
+      </c>
+      <c r="G187" s="47" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="188" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C188" s="1"/>
-      <c r="G188" s="44"/>
+      <c r="C188" s="52" t="d">
+        <v>2021-12-05</v>
+      </c>
+      <c r="D188" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="E188" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="F188" s="47">
+        <v>1</v>
+      </c>
+      <c r="G188" s="47" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="189" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C189" s="1"/>
-      <c r="G189" s="44"/>
+      <c r="C189" s="52" t="d">
+        <v>2021-12-05</v>
+      </c>
+      <c r="D189" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="E189" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="F189" s="53">
+        <v>1</v>
+      </c>
+      <c r="G189" s="47" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="190" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C190" s="1"/>
-      <c r="G190" s="44"/>
+      <c r="C190" s="52" t="d">
+        <v>2021-12-05</v>
+      </c>
+      <c r="D190" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E190" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="F190" s="53">
+        <v>1</v>
+      </c>
+      <c r="G190" s="47" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="191" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C191" s="1"/>
-      <c r="G191" s="44"/>
+      <c r="C191" s="52" t="d">
+        <v>2021-12-05</v>
+      </c>
+      <c r="D191" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="E191" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="F191" s="47">
+        <v>0.9</v>
+      </c>
+      <c r="G191" s="46" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="192" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C192" s="1"/>
-      <c r="G192" s="44"/>
+      <c r="C192" s="52" t="d">
+        <v>2021-12-05</v>
+      </c>
+      <c r="D192" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E192" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="F192" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="G192" s="47" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="193" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C193" s="1"/>
-      <c r="G193" s="44"/>
-    </row>
-    <row r="194" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C194" s="1"/>
-      <c r="G194" s="44"/>
-    </row>
-    <row r="195" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C195" s="1"/>
-      <c r="G195" s="44"/>
-    </row>
-    <row r="196" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C196" s="1"/>
-      <c r="G196" s="44"/>
-    </row>
-    <row r="197" spans="3:7" x14ac:dyDescent="0.15">
-      <c r="C197" s="1"/>
-      <c r="G197" s="44"/>
+      <c r="C193" s="52" t="d">
+        <v>2021-12-05</v>
+      </c>
+      <c r="D193" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="E193" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="F193" s="47">
+        <v>0.1</v>
+      </c>
+      <c r="G193" s="46" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="198" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C198" s="1"/>
@@ -5376,10 +5684,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -5466,15 +5774,15 @@
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="16">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D6" s="16">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
       <c r="G6" s="17">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
@@ -5484,9 +5792,7 @@
       <c r="B7" s="15">
         <v>1</v>
       </c>
-      <c r="C7" s="16">
-        <v>0.8</v>
-      </c>
+      <c r="C7" s="16"/>
       <c r="D7" s="16">
         <v>1</v>
       </c>
@@ -5497,7 +5803,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="17">
-        <v>4.8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
@@ -5511,7 +5817,7 @@
         <v>1.2</v>
       </c>
       <c r="D8" s="16">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E8" s="16">
         <v>1.2</v>
@@ -5520,30 +5826,45 @@
         <v>1.2</v>
       </c>
       <c r="G8" s="17">
-        <v>5.8</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="17">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B10" s="19">
         <v>2.5</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C10" s="20">
         <v>2.5</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D10" s="20">
         <v>2.5</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E10" s="20">
         <v>2.5</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F10" s="20">
         <v>2.5</v>
       </c>
-      <c r="G9" s="21">
-        <v>12.5</v>
+      <c r="G10" s="21">
+        <v>12.500000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>